<commit_message>
new changes to spreadsheet
</commit_message>
<xml_diff>
--- a/scripts/shstrophies/data/Mr Torren_s initial data input/Fall Awards/Field Hockey.xlsx
+++ b/scripts/shstrophies/data/Mr Torren_s initial data input/Fall Awards/Field Hockey.xlsx
@@ -20,36 +20,39 @@
     <t>Most Valuable Offense</t>
   </si>
   <si>
+    <t>Most Valuable</t>
+  </si>
+  <si>
     <t>Most Valuable Defense</t>
   </si>
   <si>
     <t xml:space="preserve">Most Improved </t>
   </si>
   <si>
+    <t>Most Valuable Offensive</t>
+  </si>
+  <si>
     <t>Captain</t>
   </si>
   <si>
+    <t>Most Valuable Defensive</t>
+  </si>
+  <si>
     <t>Most Inspirational</t>
   </si>
   <si>
+    <t>Most Improved</t>
+  </si>
+  <si>
+    <t>JV Captain</t>
+  </si>
+  <si>
+    <t>image URL</t>
+  </si>
+  <si>
     <t>imageUrl</t>
   </si>
   <si>
-    <t>Most Valuable</t>
-  </si>
-  <si>
-    <t>Most Valuable Offensive</t>
-  </si>
-  <si>
-    <t>Most Valuable Defensive</t>
-  </si>
-  <si>
-    <t>Most Improved</t>
-  </si>
-  <si>
-    <t>JV Captain</t>
-  </si>
-  <si>
     <t>DEFAULT IMAGE</t>
   </si>
   <si>
@@ -59,7 +62,49 @@
     <t>2009/2010</t>
   </si>
   <si>
-    <t>image URL</t>
+    <t>Amanda Schwartz</t>
+  </si>
+  <si>
+    <t>Evelyn Lee</t>
+  </si>
+  <si>
+    <t>Noy Shaked</t>
+  </si>
+  <si>
+    <t>2010/2011</t>
+  </si>
+  <si>
+    <t>Joanne Sturge</t>
+  </si>
+  <si>
+    <t>Ingrid Hong</t>
+  </si>
+  <si>
+    <t>2011/2012</t>
+  </si>
+  <si>
+    <t>Risha Shah</t>
+  </si>
+  <si>
+    <t>Melissa Szenda</t>
+  </si>
+  <si>
+    <t>Meeta Marathe</t>
+  </si>
+  <si>
+    <t>Monica Saripella</t>
+  </si>
+  <si>
+    <t>Lena Jewler</t>
+  </si>
+  <si>
+    <t>2012/2013</t>
+  </si>
+  <si>
+    <t>Corinne Bryan</t>
+  </si>
+  <si>
+    <t>Danielle Bruno</t>
   </si>
   <si>
     <t>Vanessa Block</t>
@@ -77,9 +122,6 @@
     <t>Jordan Leonard</t>
   </si>
   <si>
-    <t>2010/2011</t>
-  </si>
-  <si>
     <t>Kathryn Nobles</t>
   </si>
   <si>
@@ -89,54 +131,12 @@
     <t>Allison Bruno</t>
   </si>
   <si>
-    <t>2011/2012</t>
-  </si>
-  <si>
     <t>Megan Doles</t>
   </si>
   <si>
     <t>Abby Williams</t>
   </si>
   <si>
-    <t>Amanda Schwartz</t>
-  </si>
-  <si>
-    <t>Evelyn Lee</t>
-  </si>
-  <si>
-    <t>Noy Shaked</t>
-  </si>
-  <si>
-    <t>Joanne Sturge</t>
-  </si>
-  <si>
-    <t>Ingrid Hong</t>
-  </si>
-  <si>
-    <t>Risha Shah</t>
-  </si>
-  <si>
-    <t>Melissa Szenda</t>
-  </si>
-  <si>
-    <t>Meeta Marathe</t>
-  </si>
-  <si>
-    <t>Monica Saripella</t>
-  </si>
-  <si>
-    <t>Lena Jewler</t>
-  </si>
-  <si>
-    <t>2012/2013</t>
-  </si>
-  <si>
-    <t>Corinne Bryan</t>
-  </si>
-  <si>
-    <t>Danielle Bruno</t>
-  </si>
-  <si>
     <t>Rachel Leonard</t>
   </si>
   <si>
@@ -179,67 +179,70 @@
     <t>Sophie Parr</t>
   </si>
   <si>
+    <t>2015/2016</t>
+  </si>
+  <si>
+    <t>Valerie Yang (Attacker)</t>
+  </si>
+  <si>
+    <t>Tiffany Vu</t>
+  </si>
+  <si>
     <t>Vannessa Diez</t>
   </si>
   <si>
     <t>Jennifer Miller</t>
   </si>
   <si>
-    <t>2015/2016</t>
-  </si>
-  <si>
-    <t>Valerie Yang (Attacker)</t>
-  </si>
-  <si>
-    <t>Tiffany Vu</t>
-  </si>
-  <si>
     <t>Chancee Gaskin (Defender)</t>
   </si>
   <si>
+    <t>2016/2017</t>
+  </si>
+  <si>
+    <t>2017-2018</t>
+  </si>
+  <si>
+    <t>Gwen Oberhauser</t>
+  </si>
+  <si>
     <t>Anne Rollinson</t>
   </si>
   <si>
-    <t>2016/2017</t>
+    <t>Chloe Lahijanian</t>
+  </si>
+  <si>
+    <t>Judy Yang</t>
+  </si>
+  <si>
+    <t>Leila Chaudhry</t>
+  </si>
+  <si>
+    <t>Anna Schneider</t>
+  </si>
+  <si>
+    <t>Sarah Sherman</t>
   </si>
   <si>
     <t>Sabrina Clark</t>
   </si>
   <si>
-    <t>2017-2018</t>
+    <t>2018-2019</t>
+  </si>
+  <si>
+    <t>Alejandra Cordova</t>
+  </si>
+  <si>
+    <t>Lauren Yarrington</t>
   </si>
   <si>
     <t>Rachel Davey</t>
   </si>
   <si>
-    <t>Gwen Oberhauser</t>
-  </si>
-  <si>
-    <t>Chloe Lahijanian</t>
-  </si>
-  <si>
-    <t>Judy Yang</t>
-  </si>
-  <si>
-    <t>Leila Chaudhry</t>
-  </si>
-  <si>
-    <t>Anna Schneider</t>
-  </si>
-  <si>
-    <t>Sarah Sherman</t>
-  </si>
-  <si>
-    <t>2018-2019</t>
-  </si>
-  <si>
-    <t>Alejandra Cordova</t>
-  </si>
-  <si>
     <t>Tina Miller</t>
   </si>
   <si>
-    <t>Lauren Yarrington</t>
+    <t>Rima Chrisie</t>
   </si>
   <si>
     <t>Maxine Parr</t>
@@ -258,9 +261,6 @@
   </si>
   <si>
     <t>Valerie Yang</t>
-  </si>
-  <si>
-    <t>Rima Chrisie</t>
   </si>
   <si>
     <t>Kate Bossi</t>
@@ -333,30 +333,30 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
@@ -415,378 +415,378 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G1" s="4"/>
-      <c r="H1" s="5"/>
+      <c r="H1" s="6"/>
       <c r="I1" s="4"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6"/>
-      <c r="U1" s="6"/>
-      <c r="V1" s="6"/>
-      <c r="W1" s="6"/>
-      <c r="X1" s="6"/>
-      <c r="Y1" s="6"/>
-      <c r="Z1" s="6"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8"/>
+      <c r="W1" s="8"/>
+      <c r="X1" s="8"/>
+      <c r="Y1" s="8"/>
+      <c r="Z1" s="8"/>
     </row>
     <row r="2">
-      <c r="A2" s="7" t="s">
-        <v>6</v>
+      <c r="A2" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="9" t="s">
-        <v>13</v>
+      <c r="A3" s="12" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="8" t="s">
+      <c r="A4" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="8"/>
+      <c r="F4" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="13"/>
+      <c r="B5" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" s="8"/>
+      <c r="I7" s="14"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="13"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" s="8"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="13"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" s="8"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F10" s="8"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="13"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F11" s="8"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="13"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="11"/>
-      <c r="B5" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="11" t="s">
+      <c r="F12" s="8"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="8"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="13"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E14" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="F7" s="6"/>
-      <c r="I7" s="14"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="11"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="6"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="11"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="F9" s="6"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="F10" s="6"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="11"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8" t="s">
+      <c r="F14" s="8"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F15" s="8"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="10"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F16" s="8"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="10"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F17" s="8"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="10" t="s">
         <v>55</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="F11" s="6"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="11"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="F12" s="6"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="F13" s="6"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="11"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="F14" s="6"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="F15" s="6"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="7"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="F16" s="6"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="7"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="F17" s="6"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="7" t="s">
-        <v>57</v>
       </c>
       <c r="B18" s="4">
         <v>0.0</v>
       </c>
-      <c r="C18" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="D18" s="8" t="s">
+      <c r="C18" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D18" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="E18" s="8">
+      <c r="E18" s="5">
         <v>0.0</v>
       </c>
-      <c r="F18" s="6"/>
+      <c r="F18" s="8"/>
     </row>
     <row r="19">
-      <c r="A19" s="7"/>
-      <c r="C19" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
+      <c r="A19" s="10"/>
+      <c r="C19" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
     </row>
     <row r="20">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F20" s="8"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="10"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="F21" s="8"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="10"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="F22" s="8"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="B20" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="F20" s="6"/>
-    </row>
-    <row r="21">
-      <c r="A21" s="7"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="F21" s="6"/>
-    </row>
-    <row r="22">
-      <c r="A22" s="7"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="F22" s="6"/>
-    </row>
-    <row r="23">
-      <c r="A23" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="C23" s="8" t="s">
+      <c r="B23" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="D23" s="8" t="s">
+      <c r="C23" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="E23" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="F23" s="6"/>
+      <c r="D23" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="F23" s="8"/>
     </row>
     <row r="24">
-      <c r="A24" s="7"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="8" t="s">
+      <c r="A24" s="10"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="F24" s="8"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="10"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="F25" s="8"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="B26" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="F24" s="6"/>
-    </row>
-    <row r="25">
-      <c r="A25" s="7"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="F25" s="6"/>
-    </row>
-    <row r="26">
-      <c r="A26" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="B26" s="8" t="s">
+      <c r="C26" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="C26" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="D26" s="8" t="s">
+      <c r="D26" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="E26" s="8" t="s">
+      <c r="E26" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="F26" s="6"/>
+      <c r="F26" s="8"/>
     </row>
     <row r="27">
-      <c r="A27" s="9"/>
+      <c r="A27" s="12"/>
     </row>
     <row r="28">
       <c r="A28" s="18"/>
@@ -3725,194 +3725,194 @@
     <row r="1">
       <c r="A1" s="1"/>
       <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8"/>
+      <c r="W1" s="8"/>
+      <c r="X1" s="8"/>
+      <c r="Y1" s="8"/>
+      <c r="Z1" s="8"/>
+      <c r="AA1" s="8"/>
+      <c r="AB1" s="8"/>
+      <c r="AC1" s="8"/>
+      <c r="AD1" s="8"/>
+      <c r="AE1" s="8"/>
+      <c r="AF1" s="8"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6"/>
-      <c r="U1" s="6"/>
-      <c r="V1" s="6"/>
-      <c r="W1" s="6"/>
-      <c r="X1" s="6"/>
-      <c r="Y1" s="6"/>
-      <c r="Z1" s="6"/>
-      <c r="AA1" s="6"/>
-      <c r="AB1" s="6"/>
-      <c r="AC1" s="6"/>
-      <c r="AD1" s="6"/>
-      <c r="AE1" s="6"/>
-      <c r="AF1" s="6"/>
-    </row>
-    <row r="2">
-      <c r="A2" s="12" t="s">
-        <v>15</v>
-      </c>
       <c r="B2" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
+      <c r="A3" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F4" s="8"/>
-      <c r="G4" s="6"/>
+        <v>15</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="5"/>
+      <c r="G4" s="8"/>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="F5" s="8"/>
-      <c r="G5" s="6"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="8"/>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8" t="s">
-        <v>34</v>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8" t="s">
-        <v>36</v>
+      <c r="B7" s="8"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8" t="s">
-        <v>37</v>
+      <c r="B8" s="8"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8" t="s">
-        <v>40</v>
+        <v>28</v>
+      </c>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
       <c r="E10" s="14" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="F10" s="14"/>
-      <c r="G10" s="8" t="s">
+      <c r="G10" s="5" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="8" t="s">
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="5" t="s">
         <v>44</v>
       </c>
     </row>
@@ -3920,155 +3920,155 @@
       <c r="A12" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
       <c r="E12" s="14" t="s">
         <v>47</v>
       </c>
       <c r="F12" s="14"/>
-      <c r="G12" s="6"/>
+      <c r="G12" s="8"/>
     </row>
     <row r="13">
       <c r="A13" s="2"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
       <c r="E13" s="14" t="s">
         <v>49</v>
       </c>
       <c r="F13" s="14"/>
-      <c r="G13" s="6"/>
+      <c r="G13" s="8"/>
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="8" t="s">
+      <c r="B14" s="8"/>
+      <c r="C14" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="E14" s="8" t="s">
+      <c r="E14" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="F14" s="8" t="s">
+      <c r="F14" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="G14" s="8" t="s">
+      <c r="G14" s="5" t="s">
         <v>54</v>
       </c>
       <c r="I14" s="14"/>
     </row>
     <row r="15">
-      <c r="A15" s="12"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
+      <c r="A15" s="9"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
     </row>
     <row r="16">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B16" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
     </row>
     <row r="17">
-      <c r="A17" s="12"/>
-      <c r="B17" s="8" t="s">
+      <c r="A17" s="9"/>
+      <c r="B17" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
     </row>
     <row r="18">
-      <c r="A18" s="12" t="s">
+      <c r="A18" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="C18" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="D18" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="E18" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="F18" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="G18" s="5">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="B18" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="C18" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="D18" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="E18" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="F18" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="G18" s="8">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F19" s="8"/>
+      <c r="G19" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="8" t="s">
+    </row>
+    <row r="20">
+      <c r="A20" s="9"/>
+      <c r="B20" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="F19" s="6"/>
-      <c r="G19" s="8" t="s">
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="5" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="12"/>
-      <c r="B20" s="8" t="s">
+      <c r="F20" s="8"/>
+      <c r="G20" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="F20" s="6"/>
-      <c r="G20" s="8" t="s">
+    </row>
+    <row r="21">
+      <c r="A21" s="9" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="12" t="s">
+      <c r="B21" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="F21" s="6"/>
-      <c r="G21" s="8" t="s">
-        <v>73</v>
+      <c r="F21" s="8"/>
+      <c r="G21" s="5" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="22">
@@ -4079,7 +4079,7 @@
       <c r="E22" s="16"/>
       <c r="F22" s="16"/>
       <c r="G22" s="16" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="H22" s="16"/>
       <c r="I22" s="17"/>
@@ -4091,7 +4091,7 @@
     <row r="23">
       <c r="A23" s="18"/>
       <c r="G23" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="24">

</xml_diff>